<commit_message>
Normalized the values for the cases
</commit_message>
<xml_diff>
--- a/CaseData.xlsx
+++ b/CaseData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3606,7 +3606,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3642,16 +3652,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="172" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -3929,12 +3941,13 @@
   <dimension ref="A1:AB1213"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AB14" sqref="O1:AB14"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="16" max="28" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
@@ -4060,40 +4073,40 @@
         <v>1</v>
       </c>
       <c r="P2" s="2">
-        <f>SUMPRODUCT(($B$2:$B$1000=B$2:B$1000)*(LEN($B$2:$B$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>413</v>
+        <f>IFERROR(SUMPRODUCT(($B$2:$B$1250=B$2:B$1250)*(LEN($B2:$B1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($B$2:$B$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>1</v>
       </c>
       <c r="Q2" s="2">
-        <f t="shared" ref="Q2:AB2" si="0">SUMPRODUCT(($B$2:$B$1000=C$2:C$1000)*(LEN($B$2:$B$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>245</v>
+        <f t="shared" ref="Q2:AB2" si="0">IFERROR(SUMPRODUCT(($B$2:$B$1250=C$2:C$1250)*(LEN($B2:$B1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($B$2:$B$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.59322033898305082</v>
       </c>
       <c r="R2" s="2">
         <f t="shared" si="0"/>
-        <v>338</v>
+        <v>0.81840193704600483</v>
       </c>
       <c r="S2" s="2">
         <f t="shared" si="0"/>
-        <v>335</v>
+        <v>0.81113801452784506</v>
       </c>
       <c r="T2" s="2">
         <f t="shared" si="0"/>
-        <v>359</v>
+        <v>0.86924939467312345</v>
       </c>
       <c r="U2" s="2">
         <f t="shared" si="0"/>
-        <v>268</v>
+        <v>0.64891041162227603</v>
       </c>
       <c r="V2" s="2">
         <f t="shared" si="0"/>
-        <v>336</v>
+        <v>0.81355932203389836</v>
       </c>
       <c r="W2" s="2">
         <f t="shared" si="0"/>
-        <v>265</v>
+        <v>0.64164648910411626</v>
       </c>
       <c r="X2" s="2">
         <f t="shared" si="0"/>
-        <v>276</v>
+        <v>0.66828087167070216</v>
       </c>
       <c r="Y2" s="2">
         <f t="shared" si="0"/>
@@ -4150,55 +4163,55 @@
       <c r="O3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="1">
-        <f>SUMPRODUCT(($C$2:$C$1000=B$2:B$1000)*(LEN($C$2:$C$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>245</v>
-      </c>
-      <c r="Q3" s="1">
-        <f t="shared" ref="Q3:AB3" si="1">SUMPRODUCT(($C$2:$C$1000=C$2:C$1000)*(LEN($C$2:$C$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>821</v>
-      </c>
-      <c r="R3" s="1">
+      <c r="P3" s="2">
+        <f>IFERROR(SUMPRODUCT(($C$2:$C$1250=B$2:B$1250)*(LEN($C$2:$C$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($C$2:$C$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0.59322033898305082</v>
+      </c>
+      <c r="Q3" s="2">
+        <f t="shared" ref="Q3:AB3" si="1">IFERROR(SUMPRODUCT(($C$2:$C$1250=C$2:C$1250)*(LEN($C$2:$C$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($C$2:$C$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>1</v>
+      </c>
+      <c r="R3" s="2">
         <f t="shared" si="1"/>
-        <v>305</v>
-      </c>
-      <c r="S3" s="1">
+        <v>0.69634703196347036</v>
+      </c>
+      <c r="S3" s="2">
         <f t="shared" si="1"/>
-        <v>457</v>
-      </c>
-      <c r="T3" s="1">
+        <v>0.55663824604141288</v>
+      </c>
+      <c r="T3" s="2">
         <f t="shared" si="1"/>
-        <v>537</v>
-      </c>
-      <c r="U3" s="1">
+        <v>0.65408038976857485</v>
+      </c>
+      <c r="U3" s="2">
         <f t="shared" si="1"/>
-        <v>593</v>
-      </c>
-      <c r="V3" s="1">
+        <v>0.81344307270233196</v>
+      </c>
+      <c r="V3" s="2">
         <f t="shared" si="1"/>
-        <v>434</v>
-      </c>
-      <c r="W3" s="1">
+        <v>0.52862362971985388</v>
+      </c>
+      <c r="W3" s="2">
         <f t="shared" si="1"/>
-        <v>656</v>
-      </c>
-      <c r="X3" s="1">
+        <v>0.79902557856272838</v>
+      </c>
+      <c r="X3" s="2">
         <f t="shared" si="1"/>
-        <v>660</v>
-      </c>
-      <c r="Y3" s="1">
+        <v>0.80389768574908649</v>
+      </c>
+      <c r="Y3" s="2">
         <f t="shared" si="1"/>
-        <v>256</v>
-      </c>
-      <c r="Z3" s="1">
+        <v>0.62745098039215685</v>
+      </c>
+      <c r="Z3" s="2">
         <f t="shared" si="1"/>
-        <v>213</v>
-      </c>
-      <c r="AA3" s="1">
+        <v>0.55613577023498695</v>
+      </c>
+      <c r="AA3" s="2">
         <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="AB3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="AB3" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -4241,55 +4254,55 @@
       <c r="O4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="1">
-        <f>SUMPRODUCT(($D$2:$D$1000=B$2:B$1000)*(LEN($D$2:$D$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>338</v>
-      </c>
-      <c r="Q4" s="1">
-        <f t="shared" ref="Q4:AB4" si="2">SUMPRODUCT(($D$2:$D$1000=C$2:C$1000)*(LEN($D$2:$D$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>305</v>
-      </c>
-      <c r="R4" s="1">
+      <c r="P4" s="2">
+        <f>IFERROR(SUMPRODUCT(($D$2:$D$1250=B$2:B$1250)*(LEN($D$2:$D$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($D$2:$D$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0.81840193704600483</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" ref="Q4:AB4" si="2">IFERROR(SUMPRODUCT(($D$2:$D$1250=C$2:C$1250)*(LEN($D$2:$D$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($D$2:$D$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.69634703196347036</v>
+      </c>
+      <c r="R4" s="2">
         <f t="shared" si="2"/>
-        <v>438</v>
-      </c>
-      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="2">
         <f t="shared" si="2"/>
-        <v>317</v>
-      </c>
-      <c r="T4" s="1">
+        <v>0.72374429223744297</v>
+      </c>
+      <c r="T4" s="2">
         <f t="shared" si="2"/>
-        <v>348</v>
-      </c>
-      <c r="U4" s="1">
+        <v>0.79452054794520544</v>
+      </c>
+      <c r="U4" s="2">
         <f t="shared" si="2"/>
-        <v>331</v>
-      </c>
-      <c r="V4" s="1">
+        <v>0.75570776255707761</v>
+      </c>
+      <c r="V4" s="2">
         <f t="shared" si="2"/>
-        <v>306</v>
-      </c>
-      <c r="W4" s="1">
+        <v>0.69863013698630139</v>
+      </c>
+      <c r="W4" s="2">
         <f t="shared" si="2"/>
-        <v>320</v>
-      </c>
-      <c r="X4" s="1">
+        <v>0.73059360730593603</v>
+      </c>
+      <c r="X4" s="2">
         <f t="shared" si="2"/>
-        <v>339</v>
-      </c>
-      <c r="Y4" s="1">
+        <v>0.77397260273972601</v>
+      </c>
+      <c r="Y4" s="2">
         <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="Z4" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="Z4" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AA4" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4332,57 +4345,57 @@
       <c r="O5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="1">
-        <f>SUMPRODUCT(($E$2:$E$1000=B$2:B$1000)*(LEN($E$2:$E$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>335</v>
-      </c>
-      <c r="Q5" s="1">
-        <f t="shared" ref="Q5:AB5" si="3">SUMPRODUCT(($E$2:$E$1000=C$2:C$1000)*(LEN($E$2:$E$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>457</v>
-      </c>
-      <c r="R5" s="1">
+      <c r="P5" s="2">
+        <f>IFERROR(SUMPRODUCT(($E$2:$E$1250=B$2:B$1250)*(LEN($E$2:$E$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($E$2:$E$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0.81113801452784506</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" ref="Q5:AB5" si="3">IFERROR(SUMPRODUCT(($E$2:$E$1250=C$2:C$1250)*(LEN($E$2:$E$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($E$2:$E$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.55663824604141288</v>
+      </c>
+      <c r="R5" s="2">
         <f t="shared" si="3"/>
-        <v>317</v>
-      </c>
-      <c r="S5" s="1">
+        <v>0.72374429223744297</v>
+      </c>
+      <c r="S5" s="2">
         <f t="shared" si="3"/>
-        <v>999</v>
-      </c>
-      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="T5" s="2">
         <f t="shared" si="3"/>
-        <v>765</v>
-      </c>
-      <c r="U5" s="1">
+        <v>0.75412541254125409</v>
+      </c>
+      <c r="U5" s="2">
         <f t="shared" si="3"/>
-        <v>430</v>
-      </c>
-      <c r="V5" s="1">
+        <v>0.58984910836762694</v>
+      </c>
+      <c r="V5" s="2">
         <f t="shared" si="3"/>
-        <v>857</v>
-      </c>
-      <c r="W5" s="1">
+        <v>0.85396039603960394</v>
+      </c>
+      <c r="W5" s="2">
         <f t="shared" si="3"/>
-        <v>574</v>
-      </c>
-      <c r="X5" s="1">
+        <v>0.5813377374071016</v>
+      </c>
+      <c r="X5" s="2">
         <f t="shared" si="3"/>
-        <v>578</v>
-      </c>
-      <c r="Y5" s="1">
+        <v>0.58003300330033003</v>
+      </c>
+      <c r="Y5" s="2">
         <f t="shared" si="3"/>
-        <v>492</v>
-      </c>
-      <c r="Z5" s="1">
+        <v>0.82853566958698377</v>
+      </c>
+      <c r="Z5" s="2">
         <f t="shared" si="3"/>
-        <v>427</v>
-      </c>
-      <c r="AA5" s="1">
+        <v>0.75839793281653745</v>
+      </c>
+      <c r="AA5" s="2">
         <f t="shared" si="3"/>
-        <v>167</v>
-      </c>
-      <c r="AB5" s="1">
+        <v>0.60248447204968947</v>
+      </c>
+      <c r="AB5" s="2">
         <f t="shared" si="3"/>
-        <v>116</v>
+        <v>0.64615384615384619</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
@@ -4423,57 +4436,57 @@
       <c r="O6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="1">
-        <f>SUMPRODUCT(($F$2:$F$1000=B$2:B$1000)*(LEN($F$2:$F$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>359</v>
-      </c>
-      <c r="Q6" s="1">
-        <f t="shared" ref="Q6:AB6" si="4">SUMPRODUCT(($F$2:$F$1000=C$2:C$1000)*(LEN($F$2:$F$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>537</v>
-      </c>
-      <c r="R6" s="1">
+      <c r="P6" s="2">
+        <f>IFERROR(SUMPRODUCT(($F$2:$F$1250=B$2:B$1250)*(LEN($F$2:$F$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($F$2:$F$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0.86924939467312345</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" ref="Q6:AB6" si="4">IFERROR(SUMPRODUCT(($F$2:$F$1250=C$2:C$1250)*(LEN($F$2:$F$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($F$2:$F$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.65408038976857485</v>
+      </c>
+      <c r="R6" s="2">
         <f t="shared" si="4"/>
-        <v>348</v>
-      </c>
-      <c r="S6" s="1">
+        <v>0.79452054794520544</v>
+      </c>
+      <c r="S6" s="2">
         <f t="shared" si="4"/>
-        <v>765</v>
-      </c>
-      <c r="T6" s="1">
+        <v>0.75412541254125409</v>
+      </c>
+      <c r="T6" s="2">
         <f t="shared" si="4"/>
-        <v>999</v>
-      </c>
-      <c r="U6" s="1">
+        <v>1</v>
+      </c>
+      <c r="U6" s="2">
         <f t="shared" si="4"/>
-        <v>516</v>
-      </c>
-      <c r="V6" s="1">
+        <v>0.70781893004115226</v>
+      </c>
+      <c r="V6" s="2">
         <f t="shared" si="4"/>
-        <v>747</v>
-      </c>
-      <c r="W6" s="1">
+        <v>0.73432343234323427</v>
+      </c>
+      <c r="W6" s="2">
         <f t="shared" si="4"/>
-        <v>681</v>
-      </c>
-      <c r="X6" s="1">
+        <v>0.68951279933938892</v>
+      </c>
+      <c r="X6" s="2">
         <f t="shared" si="4"/>
-        <v>711</v>
-      </c>
-      <c r="Y6" s="1">
+        <v>0.72277227722772275</v>
+      </c>
+      <c r="Y6" s="2">
         <f t="shared" si="4"/>
-        <v>492</v>
-      </c>
-      <c r="Z6" s="1">
+        <v>0.82227784730913644</v>
+      </c>
+      <c r="Z6" s="2">
         <f t="shared" si="4"/>
-        <v>439</v>
-      </c>
-      <c r="AA6" s="1">
+        <v>0.77131782945736438</v>
+      </c>
+      <c r="AA6" s="2">
         <f t="shared" si="4"/>
-        <v>200</v>
-      </c>
-      <c r="AB6" s="1">
+        <v>0.73913043478260865</v>
+      </c>
+      <c r="AB6" s="2">
         <f t="shared" si="4"/>
-        <v>134</v>
+        <v>0.75641025641025639</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -4514,55 +4527,55 @@
       <c r="O7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="1">
-        <f>SUMPRODUCT(($G$2:$G$1000=B$2:B$1000)*(LEN($G$2:$G$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>268</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" ref="Q7:AB7" si="5">SUMPRODUCT(($G$2:$G$1000=C$2:C$1000)*(LEN($G$2:$G$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>593</v>
-      </c>
-      <c r="R7" s="1">
+      <c r="P7" s="2">
+        <f>IFERROR(SUMPRODUCT(($G$2:$G$1250=B$2:B$1250)*(LEN($G$2:$G$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($G$2:$G$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0.64891041162227603</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" ref="Q7:AB7" si="5">IFERROR(SUMPRODUCT(($G$2:$G$1250=C$2:C$1250)*(LEN($G$2:$G$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($G$2:$G$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.81344307270233196</v>
+      </c>
+      <c r="R7" s="2">
         <f t="shared" si="5"/>
-        <v>331</v>
-      </c>
-      <c r="S7" s="1">
+        <v>0.75570776255707761</v>
+      </c>
+      <c r="S7" s="2">
         <f t="shared" si="5"/>
-        <v>430</v>
-      </c>
-      <c r="T7" s="1">
+        <v>0.58984910836762694</v>
+      </c>
+      <c r="T7" s="2">
         <f t="shared" si="5"/>
-        <v>516</v>
-      </c>
-      <c r="U7" s="1">
+        <v>0.70781893004115226</v>
+      </c>
+      <c r="U7" s="2">
         <f t="shared" si="5"/>
-        <v>729</v>
-      </c>
-      <c r="V7" s="1">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2">
         <f t="shared" si="5"/>
-        <v>435</v>
-      </c>
-      <c r="W7" s="1">
+        <v>0.5967078189300411</v>
+      </c>
+      <c r="W7" s="2">
         <f t="shared" si="5"/>
-        <v>639</v>
-      </c>
-      <c r="X7" s="1">
+        <v>0.87654320987654322</v>
+      </c>
+      <c r="X7" s="2">
         <f t="shared" si="5"/>
-        <v>614</v>
-      </c>
-      <c r="Y7" s="1">
+        <v>0.84224965706447186</v>
+      </c>
+      <c r="Y7" s="2">
         <f t="shared" si="5"/>
-        <v>207</v>
-      </c>
-      <c r="Z7" s="1">
+        <v>0.65506329113924056</v>
+      </c>
+      <c r="Z7" s="2">
         <f t="shared" si="5"/>
-        <v>185</v>
-      </c>
-      <c r="AA7" s="1">
+        <v>0.63573883161512024</v>
+      </c>
+      <c r="AA7" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="2">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -4605,57 +4618,57 @@
       <c r="O8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="1">
-        <f>SUMPRODUCT(($H$2:$H$1000=B$2:B$1000)*(LEN($H$2:$H$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>336</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" ref="Q8:AB8" si="6">SUMPRODUCT(($H$2:$H$1000=C$2:C$1000)*(LEN($H$2:$H$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>434</v>
-      </c>
-      <c r="R8" s="1">
+      <c r="P8" s="2">
+        <f>IFERROR(SUMPRODUCT(($H$2:$H$1250=B$2:B$1250)*(LEN($H$2:$H$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($H$2:$H$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0.81355932203389836</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" ref="Q8:AB8" si="6">IFERROR(SUMPRODUCT(($H$2:$H$1250=C$2:C$1250)*(LEN($H$2:$H$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($H$2:$H$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.52862362971985388</v>
+      </c>
+      <c r="R8" s="2">
         <f t="shared" si="6"/>
-        <v>306</v>
-      </c>
-      <c r="S8" s="1">
+        <v>0.69863013698630139</v>
+      </c>
+      <c r="S8" s="2">
         <f t="shared" si="6"/>
-        <v>857</v>
-      </c>
-      <c r="T8" s="1">
+        <v>0.85396039603960394</v>
+      </c>
+      <c r="T8" s="2">
         <f t="shared" si="6"/>
-        <v>747</v>
-      </c>
-      <c r="U8" s="1">
+        <v>0.73432343234323427</v>
+      </c>
+      <c r="U8" s="2">
         <f t="shared" si="6"/>
-        <v>435</v>
-      </c>
-      <c r="V8" s="1">
+        <v>0.5967078189300411</v>
+      </c>
+      <c r="V8" s="2">
         <f t="shared" si="6"/>
-        <v>999</v>
-      </c>
-      <c r="W8" s="1">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2">
         <f t="shared" si="6"/>
-        <v>564</v>
-      </c>
-      <c r="X8" s="1">
+        <v>0.56069364161849711</v>
+      </c>
+      <c r="X8" s="2">
         <f t="shared" si="6"/>
-        <v>563</v>
-      </c>
-      <c r="Y8" s="1">
+        <v>0.56188118811881194</v>
+      </c>
+      <c r="Y8" s="2">
         <f t="shared" si="6"/>
-        <v>468</v>
-      </c>
-      <c r="Z8" s="1">
+        <v>0.78222778473091359</v>
+      </c>
+      <c r="Z8" s="2">
         <f t="shared" si="6"/>
-        <v>440</v>
-      </c>
-      <c r="AA8" s="1">
+        <v>0.79586563307493541</v>
+      </c>
+      <c r="AA8" s="2">
         <f t="shared" si="6"/>
-        <v>164</v>
-      </c>
-      <c r="AB8" s="1">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="AB8" s="2">
         <f t="shared" si="6"/>
-        <v>111</v>
+        <v>0.58461538461538465</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
@@ -4696,57 +4709,57 @@
       <c r="O9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="1">
-        <f>SUMPRODUCT(($I$2:$I$1000=B$2:B$1000)*(LEN($I$2:$I$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>265</v>
-      </c>
-      <c r="Q9" s="1">
-        <f t="shared" ref="Q9:AB9" si="7">SUMPRODUCT(($I$2:$I$1000=C$2:C$1000)*(LEN($I$2:$I$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>656</v>
-      </c>
-      <c r="R9" s="1">
+      <c r="P9" s="2">
+        <f>IFERROR(SUMPRODUCT(($I$2:$I$1250=B$2:B$1250)*(LEN($I$2:$I$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($I$2:$I$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0.64164648910411626</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" ref="Q9:AB9" si="7">IFERROR(SUMPRODUCT(($I$2:$I$1250=C$2:C$1250)*(LEN($I$2:$I$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($I$2:$I$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.79902557856272838</v>
+      </c>
+      <c r="R9" s="2">
         <f t="shared" si="7"/>
-        <v>320</v>
-      </c>
-      <c r="S9" s="1">
+        <v>0.73059360730593603</v>
+      </c>
+      <c r="S9" s="2">
         <f t="shared" si="7"/>
-        <v>574</v>
-      </c>
-      <c r="T9" s="1">
+        <v>0.5813377374071016</v>
+      </c>
+      <c r="T9" s="2">
         <f t="shared" si="7"/>
-        <v>681</v>
-      </c>
-      <c r="U9" s="1">
+        <v>0.68951279933938892</v>
+      </c>
+      <c r="U9" s="2">
         <f t="shared" si="7"/>
-        <v>639</v>
-      </c>
-      <c r="V9" s="1">
+        <v>0.87654320987654322</v>
+      </c>
+      <c r="V9" s="2">
         <f t="shared" si="7"/>
-        <v>564</v>
-      </c>
-      <c r="W9" s="1">
+        <v>0.56069364161849711</v>
+      </c>
+      <c r="W9" s="2">
         <f t="shared" si="7"/>
-        <v>999</v>
-      </c>
-      <c r="X9" s="1">
+        <v>1</v>
+      </c>
+      <c r="X9" s="2">
         <f t="shared" si="7"/>
-        <v>851</v>
-      </c>
-      <c r="Y9" s="1">
+        <v>0.856317093311313</v>
+      </c>
+      <c r="Y9" s="2">
         <f t="shared" si="7"/>
-        <v>373</v>
-      </c>
-      <c r="Z9" s="1">
+        <v>0.6378446115288221</v>
+      </c>
+      <c r="Z9" s="2">
         <f t="shared" si="7"/>
-        <v>346</v>
-      </c>
-      <c r="AA9" s="1">
+        <v>0.59637774902975416</v>
+      </c>
+      <c r="AA9" s="2">
         <f t="shared" si="7"/>
-        <v>223</v>
-      </c>
-      <c r="AB9" s="1">
+        <v>0.84232365145228216</v>
+      </c>
+      <c r="AB9" s="2">
         <f t="shared" si="7"/>
-        <v>153</v>
+        <v>0.89203084832904889</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
@@ -4787,57 +4800,57 @@
       <c r="O10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P10" s="1">
-        <f>SUMPRODUCT(($J$2:$J$1000=B$2:B$1000)*(LEN($J$2:$J$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>276</v>
-      </c>
-      <c r="Q10" s="1">
-        <f t="shared" ref="Q10:AB11" si="8">SUMPRODUCT(($J$2:$J$1000=C$2:C$1000)*(LEN($J$2:$J$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>660</v>
-      </c>
-      <c r="R10" s="1">
+      <c r="P10" s="2">
+        <f>IFERROR(SUMPRODUCT(($J$2:$J$1250=B$2:B$1250)*(LEN($J$2:$J$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($J$2:$J$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0.66828087167070216</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" ref="Q10:AB10" si="8">IFERROR(SUMPRODUCT(($J$2:$J$1250=C$2:C$1250)*(LEN($J$2:$J$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($J$2:$J$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.80389768574908649</v>
+      </c>
+      <c r="R10" s="2">
         <f t="shared" si="8"/>
-        <v>339</v>
-      </c>
-      <c r="S10" s="1">
+        <v>0.77397260273972601</v>
+      </c>
+      <c r="S10" s="2">
         <f t="shared" si="8"/>
-        <v>578</v>
-      </c>
-      <c r="T10" s="1">
+        <v>0.58003300330033003</v>
+      </c>
+      <c r="T10" s="2">
         <f t="shared" si="8"/>
-        <v>711</v>
-      </c>
-      <c r="U10" s="1">
+        <v>0.72277227722772275</v>
+      </c>
+      <c r="U10" s="2">
         <f t="shared" si="8"/>
-        <v>614</v>
-      </c>
-      <c r="V10" s="1">
+        <v>0.84224965706447186</v>
+      </c>
+      <c r="V10" s="2">
         <f t="shared" si="8"/>
-        <v>563</v>
-      </c>
-      <c r="W10" s="1">
+        <v>0.56188118811881194</v>
+      </c>
+      <c r="W10" s="2">
         <f t="shared" si="8"/>
-        <v>851</v>
-      </c>
-      <c r="X10" s="1">
+        <v>0.856317093311313</v>
+      </c>
+      <c r="X10" s="2">
         <f t="shared" si="8"/>
-        <v>999</v>
-      </c>
-      <c r="Y10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="2">
         <f t="shared" si="8"/>
-        <v>390</v>
-      </c>
-      <c r="Z10" s="1">
+        <v>0.68210262828535673</v>
+      </c>
+      <c r="Z10" s="2">
         <f t="shared" si="8"/>
-        <v>378</v>
-      </c>
-      <c r="AA10" s="1">
+        <v>0.65762273901808788</v>
+      </c>
+      <c r="AA10" s="2">
         <f t="shared" si="8"/>
-        <v>226</v>
-      </c>
-      <c r="AB10" s="1">
+        <v>0.85300207039337472</v>
+      </c>
+      <c r="AB10" s="2">
         <f t="shared" si="8"/>
-        <v>152</v>
+        <v>0.88461538461538458</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
@@ -4878,57 +4891,57 @@
       <c r="O11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="1">
-        <f>SUMPRODUCT(($K$2:$K$1000=B$2:B$1000)*(LEN($K$2:$K$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="1">
-        <f t="shared" ref="Q11:AB11" si="9">SUMPRODUCT(($K$2:$K$1000=C$2:C$1000)*(LEN($K$2:$K$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>256</v>
-      </c>
-      <c r="R11" s="1">
+      <c r="P11" s="2">
+        <f>IFERROR(SUMPRODUCT(($K$2:$K$1250=B$2:B$1250)*(LEN($K$2:$K$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($K$2:$K$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" ref="Q11:AB11" si="9">IFERROR(SUMPRODUCT(($K$2:$K$1250=C$2:C$1250)*(LEN($K$2:$K$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($K$2:$K$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.62745098039215685</v>
+      </c>
+      <c r="R11" s="2">
         <f t="shared" si="9"/>
-        <v>23</v>
-      </c>
-      <c r="S11" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="S11" s="2">
         <f t="shared" si="9"/>
-        <v>492</v>
-      </c>
-      <c r="T11" s="1">
+        <v>0.82853566958698377</v>
+      </c>
+      <c r="T11" s="2">
         <f t="shared" si="9"/>
-        <v>492</v>
-      </c>
-      <c r="U11" s="1">
+        <v>0.82227784730913644</v>
+      </c>
+      <c r="U11" s="2">
         <f t="shared" si="9"/>
-        <v>207</v>
-      </c>
-      <c r="V11" s="1">
+        <v>0.65506329113924056</v>
+      </c>
+      <c r="V11" s="2">
         <f t="shared" si="9"/>
-        <v>468</v>
-      </c>
-      <c r="W11" s="1">
+        <v>0.78222778473091359</v>
+      </c>
+      <c r="W11" s="2">
         <f t="shared" si="9"/>
-        <v>373</v>
-      </c>
-      <c r="X11" s="1">
+        <v>0.6378446115288221</v>
+      </c>
+      <c r="X11" s="2">
         <f t="shared" si="9"/>
-        <v>390</v>
-      </c>
-      <c r="Y11" s="1">
+        <v>0.68210262828535673</v>
+      </c>
+      <c r="Y11" s="2">
         <f t="shared" si="9"/>
-        <v>586</v>
-      </c>
-      <c r="Z11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="2">
         <f t="shared" si="9"/>
-        <v>476</v>
-      </c>
-      <c r="AA11" s="1">
+        <v>0.82687338501291985</v>
+      </c>
+      <c r="AA11" s="2">
         <f t="shared" si="9"/>
-        <v>193</v>
-      </c>
-      <c r="AB11" s="1">
+        <v>0.69358178053830233</v>
+      </c>
+      <c r="AB11" s="2">
         <f t="shared" si="9"/>
-        <v>127</v>
+        <v>0.68974358974358974</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
@@ -4969,57 +4982,57 @@
       <c r="O12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P12" s="1">
-        <f>SUMPRODUCT(($L$2:$L$1000=B$2:B$1000)*(LEN($L$2:$L$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="1">
-        <f t="shared" ref="Q11:AB12" si="10">SUMPRODUCT(($L$2:$L$1000=C$2:C$1000)*(LEN($L$2:$L$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>213</v>
-      </c>
-      <c r="R12" s="1">
+      <c r="P12" s="2">
+        <f>IFERROR(SUMPRODUCT(($L$2:$L$1250=B$2:B$1250)*(LEN($L$2:$L$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($L$2:$L$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" ref="Q12:AB12" si="10">IFERROR(SUMPRODUCT(($L$2:$L$1250=C$2:C$1250)*(LEN($L$2:$L$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($L$2:$L$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.55613577023498695</v>
+      </c>
+      <c r="R12" s="2">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S12" s="2">
         <f t="shared" si="10"/>
-        <v>427</v>
-      </c>
-      <c r="T12" s="1">
+        <v>0.75839793281653745</v>
+      </c>
+      <c r="T12" s="2">
         <f t="shared" si="10"/>
-        <v>439</v>
-      </c>
-      <c r="U12" s="1">
+        <v>0.77131782945736438</v>
+      </c>
+      <c r="U12" s="2">
         <f t="shared" si="10"/>
-        <v>185</v>
-      </c>
-      <c r="V12" s="1">
+        <v>0.63573883161512024</v>
+      </c>
+      <c r="V12" s="2">
         <f t="shared" si="10"/>
-        <v>440</v>
-      </c>
-      <c r="W12" s="1">
+        <v>0.79586563307493541</v>
+      </c>
+      <c r="W12" s="2">
         <f t="shared" si="10"/>
-        <v>346</v>
-      </c>
-      <c r="X12" s="1">
+        <v>0.59637774902975416</v>
+      </c>
+      <c r="X12" s="2">
         <f t="shared" si="10"/>
-        <v>378</v>
-      </c>
-      <c r="Y12" s="1">
+        <v>0.65762273901808788</v>
+      </c>
+      <c r="Y12" s="2">
         <f t="shared" si="10"/>
-        <v>476</v>
-      </c>
-      <c r="Z12" s="1">
+        <v>0.82687338501291985</v>
+      </c>
+      <c r="Z12" s="2">
         <f t="shared" si="10"/>
-        <v>561</v>
-      </c>
-      <c r="AA12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="2">
         <f t="shared" si="10"/>
-        <v>171</v>
-      </c>
-      <c r="AB12" s="1">
+        <v>0.60869565217391308</v>
+      </c>
+      <c r="AB12" s="2">
         <f t="shared" si="10"/>
-        <v>115</v>
+        <v>0.60769230769230764</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
@@ -5060,57 +5073,57 @@
       <c r="O13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P13" s="1">
-        <f>SUMPRODUCT(($M$2:$M$1000=B$2:B$1000)*(LEN($M$2:$M$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="1">
-        <f t="shared" ref="Q13:AB13" si="11">SUMPRODUCT(($M$2:$M$1000=C$2:C$1000)*(LEN($M$2:$M$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>69</v>
-      </c>
-      <c r="R13" s="1">
+      <c r="P13" s="2">
+        <f>IFERROR(SUMPRODUCT(($M$2:$M$1250=B$2:B$1250)*(LEN($M$2:$M$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($M$2:$M$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" ref="Q13:AB13" si="11">IFERROR(SUMPRODUCT(($M$2:$M$1250=C$2:C$1250)*(LEN($M$2:$M$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($M$2:$M$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0.75</v>
+      </c>
+      <c r="R13" s="2">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="S13" s="1">
+      <c r="S13" s="2">
         <f t="shared" si="11"/>
-        <v>167</v>
-      </c>
-      <c r="T13" s="1">
+        <v>0.60248447204968947</v>
+      </c>
+      <c r="T13" s="2">
         <f t="shared" si="11"/>
-        <v>200</v>
-      </c>
-      <c r="U13" s="1">
+        <v>0.73913043478260865</v>
+      </c>
+      <c r="U13" s="2">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V13" s="1">
+      <c r="V13" s="2">
         <f t="shared" si="11"/>
-        <v>164</v>
-      </c>
-      <c r="W13" s="1">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="W13" s="2">
         <f t="shared" si="11"/>
-        <v>223</v>
-      </c>
-      <c r="X13" s="1">
+        <v>0.84232365145228216</v>
+      </c>
+      <c r="X13" s="2">
         <f t="shared" si="11"/>
-        <v>226</v>
-      </c>
-      <c r="Y13" s="1">
+        <v>0.85300207039337472</v>
+      </c>
+      <c r="Y13" s="2">
         <f t="shared" si="11"/>
-        <v>193</v>
-      </c>
-      <c r="Z13" s="1">
+        <v>0.69358178053830233</v>
+      </c>
+      <c r="Z13" s="2">
         <f t="shared" si="11"/>
-        <v>171</v>
-      </c>
-      <c r="AA13" s="1">
+        <v>0.60869565217391308</v>
+      </c>
+      <c r="AA13" s="2">
         <f t="shared" si="11"/>
-        <v>270</v>
-      </c>
-      <c r="AB13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="2">
         <f t="shared" si="11"/>
-        <v>156</v>
+        <v>0.88717948717948714</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
@@ -5151,57 +5164,57 @@
       <c r="O14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P14" s="1">
-        <f>SUMPRODUCT(($N$2:$N$1000=B$2:B$1000)*(LEN($N$2:$N$1000)&gt;0)*(LEN(B$2:B$1000)&gt;0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="1">
-        <f t="shared" ref="Q14:AB14" si="12">SUMPRODUCT(($N$2:$N$1000=C$2:C$1000)*(LEN($N$2:$N$1000)&gt;0)*(LEN(C$2:C$1000)&gt;0))</f>
-        <v>0</v>
-      </c>
-      <c r="R14" s="1">
+      <c r="P14" s="2">
+        <f>IFERROR(SUMPRODUCT(($N$2:$N$1250=B$2:B$1250)*(LEN($N$2:$N$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)) / SUMPRODUCT((LEN($N$2:$N$1250)&gt;0)*(LEN(B$2:B$1250)&gt;0)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" ref="Q14:AB14" si="12">IFERROR(SUMPRODUCT(($N$2:$N$1250=C$2:C$1250)*(LEN($N$2:$N$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)) / SUMPRODUCT((LEN($N$2:$N$1250)&gt;0)*(LEN(C$2:C$1250)&gt;0)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14" s="2">
         <f t="shared" si="12"/>
-        <v>116</v>
-      </c>
-      <c r="T14" s="1">
+        <v>0.64615384615384619</v>
+      </c>
+      <c r="T14" s="2">
         <f t="shared" si="12"/>
-        <v>134</v>
-      </c>
-      <c r="U14" s="1">
+        <v>0.75641025641025639</v>
+      </c>
+      <c r="U14" s="2">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="V14" s="1">
+      <c r="V14" s="2">
         <f t="shared" si="12"/>
-        <v>111</v>
-      </c>
-      <c r="W14" s="1">
+        <v>0.58461538461538465</v>
+      </c>
+      <c r="W14" s="2">
         <f t="shared" si="12"/>
-        <v>153</v>
-      </c>
-      <c r="X14" s="1">
+        <v>0.89203084832904889</v>
+      </c>
+      <c r="X14" s="2">
         <f t="shared" si="12"/>
-        <v>152</v>
-      </c>
-      <c r="Y14" s="1">
+        <v>0.88461538461538458</v>
+      </c>
+      <c r="Y14" s="2">
         <f t="shared" si="12"/>
-        <v>127</v>
-      </c>
-      <c r="Z14" s="1">
+        <v>0.68974358974358974</v>
+      </c>
+      <c r="Z14" s="2">
         <f t="shared" si="12"/>
-        <v>115</v>
-      </c>
-      <c r="AA14" s="1">
+        <v>0.60769230769230764</v>
+      </c>
+      <c r="AA14" s="2">
         <f t="shared" si="12"/>
-        <v>156</v>
-      </c>
-      <c r="AB14" s="1">
+        <v>0.88717948717948714</v>
+      </c>
+      <c r="AB14" s="2">
         <f t="shared" si="12"/>
-        <v>178</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.2">

</xml_diff>